<commit_message>
06JUN2015-06:15 pm - Eddy
</commit_message>
<xml_diff>
--- a/COES.MVC.Intranet/Areas/Hidrologia/Reporte/RptHidrologia_00.xlsx
+++ b/COES.MVC.Intranet/Areas/Hidrologia/Reporte/RptHidrologia_00.xlsx
@@ -11,26 +11,32 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="31">
   <si>
     <t>REPORTE DE PROGRAMADO MENSUAL - QN</t>
   </si>
   <si>
-    <t>FECHA:</t>
-  </si>
-  <si>
-    <t>29/05/2015 14:15</t>
+    <t>Fecha Inicio:</t>
+  </si>
+  <si>
+    <t>ENERO - 2015</t>
+  </si>
+  <si>
+    <t>Fecha Fin:</t>
+  </si>
+  <si>
+    <t>JUNIO - 2015</t>
   </si>
   <si>
     <t>AFLUENTES</t>
   </si>
   <si>
+    <t>HUINCAUTUR</t>
+  </si>
+  <si>
     <t>NUEVO PTO EMBALSE</t>
   </si>
   <si>
-    <t>HUINCAUTUR</t>
-  </si>
-  <si>
     <t>Pto Yanango CTurbinado</t>
   </si>
   <si>
@@ -43,12 +49,12 @@
     <t>2015 - ENERO</t>
   </si>
   <si>
+    <t>131,000</t>
+  </si>
+  <si>
     <t>0,000</t>
   </si>
   <si>
-    <t>131,000</t>
-  </si>
-  <si>
     <t>10,997</t>
   </si>
   <si>
@@ -86,6 +92,18 @@
   </si>
   <si>
     <t>23,836</t>
+  </si>
+  <si>
+    <t>2015 - JUNIO</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>0,500</t>
+  </si>
+  <si>
+    <t>18,107</t>
   </si>
 </sst>
 </file>
@@ -93,7 +111,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <name val="Calibri"/>
@@ -104,12 +122,17 @@
       <name val="Calibri"/>
     </font>
     <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFFFFFF" tint="0"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="8"/>
       <name val="Calibri"/>
     </font>
   </fonts>
@@ -150,16 +173,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="1" applyFont="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" borderId="1" applyBorder="1" xfId="0"/>
+    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" borderId="1" applyBorder="1" xfId="0"/>
     <xf numFmtId="0" applyNumberFormat="1" fontId="0" applyFont="1" fillId="2" applyFill="1" borderId="1" applyBorder="1" xfId="0">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="2" applyFont="1" fillId="3" applyFill="1" borderId="1" applyBorder="1" xfId="0">
+    <xf numFmtId="0" applyNumberFormat="1" fontId="4" applyFont="1" fillId="3" applyFill="1" xfId="0">
       <alignment horizontal="centerContinuous"/>
     </xf>
-    <xf numFmtId="0" applyNumberFormat="1" fontId="3" applyFont="1" borderId="1" applyBorder="1" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -213,7 +237,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -232,10 +256,10 @@
       </c>
     </row>
     <row r="3">
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="0" t="s">
+      <c r="C3" s="3" t="s">
         <v>2</v>
       </c>
     </row>
@@ -246,95 +270,117 @@
       <c r="C4" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D4" s="3" t="s">
+    </row>
+    <row r="6">
+      <c r="B6" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="C6" s="5" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5">
-      <c r="B5" s="2" t="s">
+      <c r="D6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="E6" s="5" t="s">
         <v>8</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6">
-      <c r="B6" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="7">
       <c r="B7" s="4" t="s">
-        <v>13</v>
+        <v>9</v>
       </c>
       <c r="C7" s="4" t="s">
         <v>10</v>
       </c>
       <c r="D7" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="4" t="s">
+    </row>
+    <row r="9">
+      <c r="B9" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="8">
-      <c r="B8" s="4" t="s">
+      <c r="C9" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D8" s="4" t="s">
+      <c r="D9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E8" s="4" t="s">
+    </row>
+    <row r="10">
+      <c r="B10" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="9">
-      <c r="B9" s="4" t="s">
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D9" s="4" t="s">
+      <c r="D10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="4" t="s">
+    </row>
+    <row r="11">
+      <c r="B11" s="2" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="10">
-      <c r="B10" s="4" t="s">
+      <c r="C11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" s="4" t="s">
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="E10" s="4" t="s">
+    </row>
+    <row r="12">
+      <c r="B12" s="2" t="s">
         <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>